<commit_message>
adding sector 0 = consumption
</commit_message>
<xml_diff>
--- a/1-Data-Codes/0-Raw_Data/sectors.xlsx
+++ b/1-Data-Codes/0-Raw_Data/sectors.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="32">
   <si>
     <t>final_sector</t>
   </si>
@@ -105,6 +105,21 @@
   </si>
   <si>
     <t>Other Services (except Public Administration)</t>
+  </si>
+  <si>
+    <t>Final consumption expenditure by households</t>
+  </si>
+  <si>
+    <t>Final consumption expenditure by non-profit organisations serving households (NPISH)</t>
+  </si>
+  <si>
+    <t>Final consumption expenditure by government</t>
+  </si>
+  <si>
+    <t>Gross fixed capital formation</t>
+  </si>
+  <si>
+    <t>Changes in inventories and valuables</t>
   </si>
 </sst>
 </file>
@@ -422,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D91"/>
+  <dimension ref="A1:D96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1708,6 +1723,61 @@
         <v>5</v>
       </c>
     </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A92">
+        <v>0</v>
+      </c>
+      <c r="C92">
+        <v>37</v>
+      </c>
+      <c r="D92" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A93">
+        <v>0</v>
+      </c>
+      <c r="C93">
+        <v>38</v>
+      </c>
+      <c r="D93" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A94">
+        <v>0</v>
+      </c>
+      <c r="C94">
+        <v>39</v>
+      </c>
+      <c r="D94" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A95">
+        <v>0</v>
+      </c>
+      <c r="C95">
+        <v>41</v>
+      </c>
+      <c r="D95" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A96">
+        <v>0</v>
+      </c>
+      <c r="C96">
+        <v>42</v>
+      </c>
+      <c r="D96" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:D91">
     <sortCondition ref="A2:A91"/>

</xml_diff>